<commit_message>
PROS-11758 DiageoIN Brand Presence Bug fix for non POP and PROP stores
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOIN/Data/Template.xlsx
+++ b/Projects/DIAGEOIN/Data/Template.xlsx
@@ -183,17 +183,17 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="43.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1021" min="5" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5384615384615"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.3765182186235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1021" min="5" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>